<commit_message>
frontend dev version. backend recommendations fix
</commit_message>
<xml_diff>
--- a/backend/Basic data.xlsx
+++ b/backend/Basic data.xlsx
@@ -3,11 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Introduction" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Instructions" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Attitudes" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Values" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Aspects" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="Introduction" sheetId="1" r:id="rId5"/>
+    <sheet state="visible" name="Instructions" sheetId="2" r:id="rId6"/>
+    <sheet state="visible" name="Attitudes" sheetId="3" r:id="rId7"/>
+    <sheet state="visible" name="Values" sheetId="4" r:id="rId8"/>
+    <sheet state="visible" name="Aspects" sheetId="5" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="155">
   <si>
     <t>en</t>
   </si>
@@ -31,7 +31,7 @@
 If successful, this project should become a push for the beginning of new, long—term, and strong relationships.
 To do this, I propose defining your values — and based on this, the algorithm will select similar participants.
 Since, as a rule, different people put different meanings into the same words, I suggest you not only choose values ​​that are close to yours, but also choose the meanings that you put into these terms.
-Due to this approach, finding suitable users may take quite a while — and will certainly take time in the early stages, until a sufficient number of users have been recruited. I hope this won't discourage you.
+Due to this approach, finding suitable users may take quite a while — especially in the early stages, until a sufficient number of users participate. I hope this won't discourage you.
 If you want to know the reasons behind the choice of terms denoting values, here is the position from which I follow:
 1. Reality exists independently of us and is knowable through experience. It can be understood as a set of all possible descriptive statements that denote either the very fact of our experience, or logically necessarily follow from the totality of facts.
 2. Another type of statements are evaluative. We make evaluative statements about what we think reality should be like. Evaluative statements can take forms such as "X is good/bad, right/wrong" and "X should/should not be done".
@@ -60,7 +60,7 @@
 В случае успеха, этот проект должен стать толчком для начала новых длительных и крепких отношений.
 Для этого предлагаю определить ваши ценности — и на основе этого алгоритм подберёт похожих участников.
 Поскольку, как-правило, разные люди вкладывают разный смысл в одни и те же слова — я предлагаю вам не только выбрать ценности, близкие вашим, но и выбрать те смыслы, которые вы вкладываете в эти термины.
-В связи с таким подходом, поиск подходящих пользователей может занять довольно продолжительное время — и наверняка займёт на раннем этапе — пока не наберётся достаточное количество пользователей. Надеюсь, это вас не отпугнёт.
+В связи с таким подходом, поиск подходящих пользователей может занять довольно продолжительное время — особенно на раннем этапе — пока не наберётся достаточное количество пользователей. Надеюсь, это вас не отпугнёт.
 Если вы хотите узнать, чем обусловлен выбор терминов, обозначающих ценности — вот позиция, из которой я исхожу:
 1. Реальность существует независимо от нас и познаваема посредством опыта. Её можно понимать как совокупность всех возможных описательных утверждений, которые обозначают либо сам факт нашего опыта, либо логически необходимо следуют из всей совокупности фактов.
 2. Ещё один тип утверждений — оценочные. Мы делаем оценочные утверждения о том, какой, по нашему мнению, должна быть реальность. Оценочные утверждения могут иметь такие формы, как «X — это хорошо/плохо, правильно/неправильно» и «следует / не следует сделать X».
@@ -101,22 +101,22 @@
 На третьем этапе выберете утверждение, которое характеризует ваше отношение к ценностям в целом.</t>
   </si>
   <si>
-    <t>I only care about my future: I would like more {positive values} and less {negative_values} in my life. I don't care about other people's futures.</t>
+    <t>I only care about my own future: I want there to be more good things and lees bad things in my life.</t>
   </si>
   <si>
-    <t>Меня волнует только моё будущее: я хотел(а) бы больше {positive values} и меньше {negative_values} в своей жизни. Будущее других людей меня не волнует.</t>
+    <t>Меня волнует только моё будущее: я хотел(а) бы больше хорошего и меньше плохого в своей жизни.</t>
   </si>
   <si>
-    <t>I care about my future and the future of people like me: I would like more {positive values} and less {negative_values} in my life and in the lives of any people with the same values.</t>
+    <t>I care about my future and the future of people like me: I would like to have more good things and fewer bad thigs in my life and in the lives of people with similar values.</t>
   </si>
   <si>
-    <t>Меня волнует моё будущее и будущее таких же, как я: я хотел бы больше {positive values} и меньше {negative_values} в своей жизни и в жизни людей с такими же ценностями.</t>
+    <t>Меня волнует моё будущее и будущее таких же, как я: я хотел(а) бы больше хорошего и меньше плохого в своей жизни и в жизни людей с такими же ценностями.</t>
   </si>
   <si>
-    <t>I care about the future of all people: I would like all people to have more {positive values} and less {negative_values}.</t>
+    <t>I care about the future of all people: I would like all people to have more good things and less bad things in their life.</t>
   </si>
   <si>
-    <t>Меня волнует будущее всех людей: я хотел(а) бы, чтобы в жизни всех людей было больше {positive values} и меньше {negative_values}.</t>
+    <t>Меня волнует будущее всех людей: я хотел(а) бы, чтобы в жизни всех людей было больше хорошего и меньше плохого.</t>
   </si>
   <si>
     <t>Pleasure</t>
@@ -224,18 +224,6 @@
     <t>Я думаю, что удовольствие может быть интеллектуальным, и/или эмоциональным, и/или моральным.</t>
   </si>
   <si>
-    <t>absence pain/suffering</t>
-  </si>
-  <si>
-    <t>отсутствие боли/страданий</t>
-  </si>
-  <si>
-    <t>I think pleasure implies the absence of pain/suffering.</t>
-  </si>
-  <si>
-    <t>Я думаю, что удовольствие предполагает отсутствие боли/страданий.</t>
-  </si>
-  <si>
     <t>emotional well-being, low anxiety</t>
   </si>
   <si>
@@ -254,10 +242,10 @@
     <t>стабильность</t>
   </si>
   <si>
-    <t>I think comfort is stability.</t>
+    <t>I think comfort implies stability.</t>
   </si>
   <si>
-    <t>Я думаю, что комфорт — это стабильность.</t>
+    <t>Я думаю, что комфорт предполагает стабильность.</t>
   </si>
   <si>
     <t>only long-term, stable</t>
@@ -416,18 +404,6 @@
     <t>Я считаю, что статус — это достоинство, признание и уважение со стороны других.</t>
   </si>
   <si>
-    <t>imposing will</t>
-  </si>
-  <si>
-    <t>навязывание воли</t>
-  </si>
-  <si>
-    <t>I think power is imposing will.</t>
-  </si>
-  <si>
-    <t>Я думаю, что власть — это навязывание воли.</t>
-  </si>
-  <si>
     <t>influencing outcomes/decisions/behavior</t>
   </si>
   <si>
@@ -512,6 +488,18 @@
     <t>Я думаю, что насилие может исходить от социальных систем / институтов / культуры.</t>
   </si>
   <si>
+    <t>facts and logic</t>
+  </si>
+  <si>
+    <t>факты и логика</t>
+  </si>
+  <si>
+    <t>I think that truth is based on facts and logic.</t>
+  </si>
+  <si>
+    <t>Я думаю, что истина опирается на факты и логику.</t>
+  </si>
+  <si>
     <t>corresponds to reality</t>
   </si>
   <si>
@@ -546,18 +534,6 @@
   </si>
   <si>
     <t>Я думаю, что свобода — это отсутствие принуждения или ограничения в выборе или действии (со стороны других).</t>
-  </si>
-  <si>
-    <t>power over oneself</t>
-  </si>
-  <si>
-    <t>власть над собой</t>
-  </si>
-  <si>
-    <t>I think freedom is power over oneself.</t>
-  </si>
-  <si>
-    <t>Я думаю, что свобода — это власть над собой.</t>
   </si>
   <si>
     <t>implies responsibility</t>
@@ -686,6 +662,10 @@
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1506,7 +1486,7 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>47</v>
@@ -1576,7 +1556,7 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>55</v>
@@ -1591,6 +1571,12 @@
         <v>58</v>
       </c>
       <c r="F6" s="3"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
@@ -1626,8 +1612,7 @@
         <v>62</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="11"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
@@ -1667,10 +1652,8 @@
         <v>66</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="H8" s="5"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
@@ -1692,7 +1675,7 @@
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>67</v>
@@ -1707,8 +1690,11 @@
         <v>70</v>
       </c>
       <c r="F9" s="3"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
@@ -1786,12 +1772,6 @@
         <v>78</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
@@ -1847,7 +1827,7 @@
     </row>
     <row r="13">
       <c r="A13" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>83</v>
@@ -1897,6 +1877,12 @@
         <v>90</v>
       </c>
       <c r="F14" s="3"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
       <c r="M14" s="11"/>
       <c r="N14" s="11"/>
       <c r="O14" s="11"/>
@@ -1917,7 +1903,7 @@
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>91</v>
@@ -1999,7 +1985,7 @@
     </row>
     <row r="17">
       <c r="A17" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>99</v>
@@ -2081,7 +2067,7 @@
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>107</v>
@@ -2095,7 +2081,7 @@
       <c r="E19" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F19" s="3"/>
+      <c r="F19" s="7"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
@@ -2245,7 +2231,7 @@
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>123</v>
@@ -2286,7 +2272,7 @@
     </row>
     <row r="24">
       <c r="A24" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>127</v>
@@ -2368,7 +2354,7 @@
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>135</v>
@@ -2409,7 +2395,7 @@
     </row>
     <row r="27">
       <c r="A27" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>139</v>
@@ -2450,7 +2436,7 @@
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>143</v>
@@ -2465,7 +2451,7 @@
         <v>146</v>
       </c>
       <c r="F28" s="7"/>
-      <c r="G28" s="11"/>
+      <c r="G28" s="10"/>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
@@ -2534,7 +2520,7 @@
       <c r="A30" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="3" t="s">
         <v>151</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -2546,7 +2532,7 @@
       <c r="E30" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="F30" s="7"/>
+      <c r="F30" s="10"/>
       <c r="G30" s="10"/>
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
@@ -2572,23 +2558,13 @@
       <c r="AC30" s="11"/>
     </row>
     <row r="31">
-      <c r="A31" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="10"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
       <c r="J31" s="11"/>
@@ -2613,23 +2589,13 @@
       <c r="AC31" s="11"/>
     </row>
     <row r="32">
-      <c r="A32" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
       <c r="J32" s="11"/>
@@ -31452,68 +31418,6 @@
       <c r="AB961" s="11"/>
       <c r="AC961" s="11"/>
     </row>
-    <row r="962">
-      <c r="A962" s="11"/>
-      <c r="B962" s="11"/>
-      <c r="C962" s="11"/>
-      <c r="D962" s="11"/>
-      <c r="E962" s="11"/>
-      <c r="F962" s="11"/>
-      <c r="G962" s="11"/>
-      <c r="H962" s="11"/>
-      <c r="I962" s="11"/>
-      <c r="J962" s="11"/>
-      <c r="K962" s="11"/>
-      <c r="L962" s="11"/>
-      <c r="M962" s="11"/>
-      <c r="N962" s="11"/>
-      <c r="O962" s="11"/>
-      <c r="P962" s="11"/>
-      <c r="Q962" s="11"/>
-      <c r="R962" s="11"/>
-      <c r="S962" s="11"/>
-      <c r="T962" s="11"/>
-      <c r="U962" s="11"/>
-      <c r="V962" s="11"/>
-      <c r="W962" s="11"/>
-      <c r="X962" s="11"/>
-      <c r="Y962" s="11"/>
-      <c r="Z962" s="11"/>
-      <c r="AA962" s="11"/>
-      <c r="AB962" s="11"/>
-      <c r="AC962" s="11"/>
-    </row>
-    <row r="963">
-      <c r="A963" s="11"/>
-      <c r="B963" s="11"/>
-      <c r="C963" s="11"/>
-      <c r="D963" s="11"/>
-      <c r="E963" s="11"/>
-      <c r="F963" s="11"/>
-      <c r="G963" s="11"/>
-      <c r="H963" s="11"/>
-      <c r="I963" s="11"/>
-      <c r="J963" s="11"/>
-      <c r="K963" s="11"/>
-      <c r="L963" s="11"/>
-      <c r="M963" s="11"/>
-      <c r="N963" s="11"/>
-      <c r="O963" s="11"/>
-      <c r="P963" s="11"/>
-      <c r="Q963" s="11"/>
-      <c r="R963" s="11"/>
-      <c r="S963" s="11"/>
-      <c r="T963" s="11"/>
-      <c r="U963" s="11"/>
-      <c r="V963" s="11"/>
-      <c r="W963" s="11"/>
-      <c r="X963" s="11"/>
-      <c r="Y963" s="11"/>
-      <c r="Z963" s="11"/>
-      <c r="AA963" s="11"/>
-      <c r="AB963" s="11"/>
-      <c r="AC963" s="11"/>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>